<commit_message>
Updated weekly Project Plan
</commit_message>
<xml_diff>
--- a/doc/Project Plan_weekly.xlsx
+++ b/doc/Project Plan_weekly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\School\Semester2\Project\6.2A_MandyCortis_Project_Git\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E32638E-F9C0-4512-9E16-EB096A619B41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C769A-92F0-4083-B73D-2C5AD196B07D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
+    <workbookView xWindow="38280" yWindow="9825" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>Create an account</t>
   </si>
@@ -251,12 +251,6 @@
   </si>
   <si>
     <t>Wk14</t>
-  </si>
-  <si>
-    <t>Download Satellite images</t>
-  </si>
-  <si>
-    <t>Compare images</t>
   </si>
   <si>
     <t>Tutorial / Training</t>
@@ -269,7 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,13 +275,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -529,11 +516,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37548FD9-318C-4A7A-9098-287F0A874FE1}">
   <dimension ref="B1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:J21"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +943,7 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1021,10 +1008,10 @@
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
+      <c r="B8" s="25"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1149,10 +1136,10 @@
       <c r="Q15" s="14"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
+      <c r="B16" s="25"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="25" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1204,7 +1191,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="1"/>
@@ -1225,6 +1212,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="1"/>
@@ -1256,10 +1244,10 @@
       <c r="Q22" s="14"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
+      <c r="B23" s="25"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1344,17 +1332,17 @@
       <c r="Q28" s="14"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
+      <c r="B29" s="25"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="10"/>
@@ -1374,7 +1362,7 @@
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1400,7 +1388,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="27"/>
+      <c r="H33" s="26"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
@@ -1422,8 +1410,8 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="1"/>
@@ -1444,7 +1432,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="27"/>
+      <c r="L35" s="26"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
       <c r="O35" s="1"/>
@@ -1470,22 +1458,22 @@
       <c r="Q36" s="14"/>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="P37" s="25"/>
-      <c r="Q37" s="25"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="25" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1590,10 +1578,10 @@
       <c r="Q43" s="14"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B44" s="26"/>
+      <c r="B44" s="25"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1658,25 +1646,25 @@
       <c r="Q48" s="14"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B49" s="24"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="25"/>
-      <c r="P49" s="25"/>
-      <c r="Q49" s="25"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="24"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1686,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62287C0-7FD6-48A5-9514-03B257F96545}">
   <dimension ref="B1:Q48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X46" sqref="X46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,8 +1789,8 @@
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="19"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -1821,8 +1809,8 @@
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="19"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -1841,8 +1829,8 @@
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -1885,7 +1873,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -1905,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -1926,18 +1914,18 @@
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="20"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="26"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
@@ -2029,10 +2017,10 @@
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
@@ -2049,10 +2037,10 @@
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
@@ -2069,10 +2057,10 @@
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
@@ -2089,10 +2077,10 @@
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
@@ -2254,11 +2242,11 @@
         <v>75</v>
       </c>
       <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
@@ -2274,11 +2262,11 @@
         <v>76</v>
       </c>
       <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
@@ -2467,7 +2455,7 @@
       <c r="L42" s="19"/>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
-      <c r="O42" s="23"/>
+      <c r="O42" s="22"/>
       <c r="P42" s="19"/>
       <c r="Q42" s="20"/>
     </row>
@@ -2555,7 +2543,7 @@
       <c r="Q47" s="20"/>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="24"/>
+      <c r="B48" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2564,21 +2552,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100504F0EFF1BE61D46A34440DDC749B165" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6861fccdae819c068e3d2675729df3bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29ddf0ed-477c-451e-8755-cfaffaaa5733" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fc745dc185d8196f008ac861e10f643" ns2:_="">
     <xsd:import namespace="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
@@ -2710,31 +2683,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD7FEF4-E84B-468B-9D19-73896C646B9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2750,4 +2714,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KU5 - Updated Project Plan
</commit_message>
<xml_diff>
--- a/doc/Project Plan_weekly.xlsx
+++ b/doc/Project Plan_weekly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\School\Semester2\Project\6.2A_MandyCortis_Project_Git\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1C769A-92F0-4083-B73D-2C5AD196B07D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3570AC6C-0A5C-4F17-944D-842BBED20BEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="9825" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>Create an account</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>Setup Environment / Code</t>
+  </si>
+  <si>
+    <t>6th April</t>
+  </si>
+  <si>
+    <t>Wk15</t>
+  </si>
+  <si>
+    <t>WK15</t>
   </si>
 </sst>
 </file>
@@ -835,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37548FD9-318C-4A7A-9098-287F0A874FE1}">
-  <dimension ref="B1:Q49"/>
+  <dimension ref="B1:R49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:I32"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +856,7 @@
     <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>50</v>
       </c>
@@ -867,32 +876,35 @@
         <v>55</v>
       </c>
       <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>59</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
@@ -941,13 +953,16 @@
       <c r="Q3" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -964,10 +979,11 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="14"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -984,10 +1000,11 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="14"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -1004,18 +1021,19 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="14"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P7" s="19"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="25"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -1032,10 +1050,11 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="14"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="14"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -1052,10 +1071,11 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="14"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P11" s="1"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="14"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -1072,10 +1092,11 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="7"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1092,10 +1113,11 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="14"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="14"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>8</v>
@@ -1112,10 +1134,11 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="14"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="14"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
         <v>44</v>
@@ -1132,18 +1155,19 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="14"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="14"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="25"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -1160,10 +1184,11 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="14"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -1180,10 +1205,11 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="14"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="14"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
         <v>16</v>
@@ -1194,16 +1220,17 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="8"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="14"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P20" s="1"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="14"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -1215,15 +1242,16 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="1"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="14"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P21" s="1"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="14"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1239,19 +1267,20 @@
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="8"/>
+      <c r="O22" s="19"/>
       <c r="P22" s="8"/>
-      <c r="Q22" s="14"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q22" s="8"/>
+      <c r="R22" s="14"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="1" t="s">
         <v>20</v>
@@ -1262,16 +1291,17 @@
       <c r="G25" s="1"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="1"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="14"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="14"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="1" t="s">
         <v>21</v>
@@ -1282,16 +1312,17 @@
       <c r="G26" s="1"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="14"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P26" s="1"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="14"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
         <v>22</v>
@@ -1302,16 +1333,17 @@
       <c r="G27" s="1"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="1"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="14"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P27" s="1"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="14"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -1322,24 +1354,25 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="9"/>
+      <c r="J28" s="1"/>
       <c r="K28" s="9"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="19"/>
+      <c r="N28" s="1"/>
       <c r="O28" s="19"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="14"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P28" s="19"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="1" t="s">
         <v>75</v>
@@ -1352,14 +1385,15 @@
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
-      <c r="L31" s="1"/>
+      <c r="L31" s="10"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="14"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="14"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="1" t="s">
         <v>76</v>
@@ -1372,14 +1406,15 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
-      <c r="L32" s="1"/>
+      <c r="L32" s="10"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="14"/>
-    </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="14"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
         <v>11</v>
@@ -1394,12 +1429,13 @@
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
-      <c r="N33" s="1"/>
+      <c r="N33" s="10"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="14"/>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="14"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -1410,16 +1446,17 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="26"/>
+      <c r="J34" s="1"/>
       <c r="K34" s="26"/>
-      <c r="L34" s="10"/>
+      <c r="L34" s="26"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="1"/>
+      <c r="N34" s="10"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="14"/>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P34" s="1"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="14"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
         <v>45</v>
@@ -1432,14 +1469,15 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="10"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="26"/>
       <c r="N35" s="10"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="14"/>
-    </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O35" s="10"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="14"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1451,13 +1489,14 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="10"/>
+      <c r="M36" s="1"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="14"/>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P36" s="10"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="14"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -1469,15 +1508,16 @@
       <c r="J37" s="24"/>
       <c r="K37" s="24"/>
       <c r="L37" s="24"/>
-      <c r="P37" s="24"/>
+      <c r="M37" s="24"/>
       <c r="Q37" s="24"/>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="24"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
         <v>46</v>
@@ -1492,12 +1532,13 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="11"/>
+      <c r="N39" s="1"/>
       <c r="O39" s="11"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="14"/>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P39" s="11"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="14"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="1" t="s">
         <v>47</v>
@@ -1512,12 +1553,13 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="N40" s="11"/>
+      <c r="N40" s="1"/>
       <c r="O40" s="11"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="14"/>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P40" s="11"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="14"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="1" t="s">
         <v>48</v>
@@ -1533,11 +1575,12 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="14"/>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O41" s="1"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="14"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="1" t="s">
         <v>49</v>
@@ -1553,11 +1596,12 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="17"/>
-      <c r="Q42" s="14"/>
-    </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O42" s="1"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="14"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="1" t="s">
         <v>18</v>
@@ -1573,19 +1617,20 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="17"/>
-      <c r="Q43" s="14"/>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O43" s="1"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="14"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="25"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="1" t="s">
         <v>25</v>
@@ -1602,10 +1647,11 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="14"/>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P46" s="1"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="14"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="1" t="s">
         <v>26</v>
@@ -1622,10 +1668,11 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="14"/>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P47" s="1"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="14"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="1" t="s">
         <v>27</v>
@@ -1642,10 +1689,11 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="14"/>
-    </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P48" s="1"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="14"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="23"/>
       <c r="C49" s="24"/>
       <c r="D49" s="24"/>
@@ -1662,6 +1710,7 @@
       <c r="O49" s="24"/>
       <c r="P49" s="24"/>
       <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1672,19 +1721,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62287C0-7FD6-48A5-9514-03B257F96545}">
-  <dimension ref="B1:Q48"/>
+  <dimension ref="B1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>50</v>
       </c>
@@ -1704,32 +1765,35 @@
         <v>55</v>
       </c>
       <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>59</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
@@ -1778,13 +1842,16 @@
       <c r="Q3" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -1802,9 +1869,10 @@
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
-      <c r="Q5" s="20"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q5" s="19"/>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -1822,9 +1890,10 @@
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q6" s="19"/>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -1842,9 +1911,10 @@
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
-      <c r="Q7" s="20"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q7" s="19"/>
+      <c r="R7" s="20"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
       <c r="D8" s="19"/>
@@ -1860,14 +1930,15 @@
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
       <c r="P8" s="19"/>
-      <c r="Q8" s="20"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q8" s="19"/>
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -1885,9 +1956,10 @@
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
-      <c r="Q10" s="20"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q10" s="19"/>
+      <c r="R10" s="20"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -1905,9 +1977,10 @@
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
-      <c r="Q11" s="20"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q11" s="19"/>
+      <c r="R11" s="20"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -1918,16 +1991,17 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="26"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="26"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P12" s="26"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="26"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1945,9 +2019,10 @@
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
-      <c r="Q13" s="20"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q13" s="19"/>
+      <c r="R13" s="20"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>8</v>
@@ -1965,9 +2040,10 @@
       <c r="N14" s="19"/>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
-      <c r="Q14" s="20"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q14" s="19"/>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
         <v>44</v>
@@ -1985,9 +2061,10 @@
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
       <c r="P15" s="19"/>
-      <c r="Q15" s="20"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q15" s="19"/>
+      <c r="R15" s="20"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
       <c r="D16" s="19"/>
@@ -2003,14 +2080,15 @@
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
       <c r="P16" s="19"/>
-      <c r="Q16" s="20"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q16" s="19"/>
+      <c r="R16" s="20"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -2021,16 +2099,17 @@
       <c r="G18" s="8"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="19"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
       <c r="O18" s="19"/>
       <c r="P18" s="19"/>
-      <c r="Q18" s="20"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q18" s="19"/>
+      <c r="R18" s="20"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -2041,16 +2120,17 @@
       <c r="G19" s="8"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="19"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
       <c r="O19" s="19"/>
       <c r="P19" s="19"/>
-      <c r="Q19" s="20"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q19" s="19"/>
+      <c r="R19" s="20"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
         <v>16</v>
@@ -2061,16 +2141,17 @@
       <c r="G20" s="26"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="19"/>
+      <c r="J20" s="8"/>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
       <c r="P20" s="19"/>
-      <c r="Q20" s="20"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q20" s="19"/>
+      <c r="R20" s="20"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -2081,16 +2162,17 @@
       <c r="G21" s="1"/>
       <c r="H21" s="26"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="19"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
       <c r="P21" s="19"/>
-      <c r="Q21" s="20"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q21" s="19"/>
+      <c r="R21" s="20"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2108,9 +2190,10 @@
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
       <c r="P22" s="19"/>
-      <c r="Q22" s="20"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q22" s="19"/>
+      <c r="R22" s="20"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
       <c r="D23" s="19"/>
@@ -2126,14 +2209,15 @@
       <c r="N23" s="19"/>
       <c r="O23" s="19"/>
       <c r="P23" s="19"/>
-      <c r="Q23" s="20"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q23" s="19"/>
+      <c r="R23" s="20"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="1" t="s">
         <v>20</v>
@@ -2151,9 +2235,10 @@
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
-      <c r="Q25" s="20"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q25" s="19"/>
+      <c r="R25" s="20"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="1" t="s">
         <v>21</v>
@@ -2171,9 +2256,10 @@
       <c r="N26" s="19"/>
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
-      <c r="Q26" s="20"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q26" s="19"/>
+      <c r="R26" s="20"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
         <v>22</v>
@@ -2191,9 +2277,10 @@
       <c r="N27" s="19"/>
       <c r="O27" s="19"/>
       <c r="P27" s="19"/>
-      <c r="Q27" s="20"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q27" s="19"/>
+      <c r="R27" s="20"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -2211,9 +2298,10 @@
       <c r="N28" s="19"/>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
-      <c r="Q28" s="20"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q28" s="19"/>
+      <c r="R28" s="20"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
       <c r="D29" s="19"/>
@@ -2229,14 +2317,15 @@
       <c r="N29" s="19"/>
       <c r="O29" s="19"/>
       <c r="P29" s="19"/>
-      <c r="Q29" s="20"/>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q29" s="19"/>
+      <c r="R29" s="20"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="1" t="s">
         <v>75</v>
@@ -2247,16 +2336,17 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
-      <c r="J31" s="19"/>
+      <c r="J31" s="10"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
       <c r="P31" s="19"/>
-      <c r="Q31" s="20"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q31" s="19"/>
+      <c r="R31" s="20"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="1" t="s">
         <v>76</v>
@@ -2267,16 +2357,17 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
-      <c r="J32" s="19"/>
+      <c r="J32" s="10"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
       <c r="O32" s="19"/>
       <c r="P32" s="19"/>
-      <c r="Q32" s="20"/>
-    </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q32" s="19"/>
+      <c r="R32" s="20"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
         <v>11</v>
@@ -2294,9 +2385,10 @@
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
-      <c r="Q33" s="20"/>
-    </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q33" s="19"/>
+      <c r="R33" s="20"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -2314,9 +2406,10 @@
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
-      <c r="Q34" s="20"/>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q34" s="19"/>
+      <c r="R34" s="20"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
         <v>45</v>
@@ -2334,9 +2427,10 @@
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
-      <c r="Q35" s="20"/>
-    </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q35" s="19"/>
+      <c r="R35" s="20"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
       <c r="D36" s="19"/>
@@ -2352,14 +2446,15 @@
       <c r="N36" s="19"/>
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
-      <c r="Q36" s="20"/>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q36" s="19"/>
+      <c r="R36" s="20"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
         <v>46</v>
@@ -2377,9 +2472,10 @@
       <c r="N38" s="19"/>
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
-      <c r="Q38" s="20"/>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q38" s="19"/>
+      <c r="R38" s="20"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
         <v>47</v>
@@ -2397,9 +2493,10 @@
       <c r="N39" s="19"/>
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
-      <c r="Q39" s="20"/>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q39" s="19"/>
+      <c r="R39" s="20"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="1" t="s">
         <v>48</v>
@@ -2417,9 +2514,10 @@
       <c r="N40" s="19"/>
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
-      <c r="Q40" s="20"/>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q40" s="19"/>
+      <c r="R40" s="20"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="1" t="s">
         <v>49</v>
@@ -2437,9 +2535,10 @@
       <c r="N41" s="19"/>
       <c r="O41" s="19"/>
       <c r="P41" s="19"/>
-      <c r="Q41" s="20"/>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q41" s="19"/>
+      <c r="R41" s="20"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="1" t="s">
         <v>18</v>
@@ -2455,11 +2554,12 @@
       <c r="L42" s="19"/>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="20"/>
-    </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O42" s="19"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="20"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="1"/>
       <c r="D43" s="19"/>
@@ -2475,14 +2575,15 @@
       <c r="N43" s="19"/>
       <c r="O43" s="19"/>
       <c r="P43" s="19"/>
-      <c r="Q43" s="20"/>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q43" s="19"/>
+      <c r="R43" s="20"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="1" t="s">
         <v>25</v>
@@ -2500,9 +2601,10 @@
       <c r="N45" s="19"/>
       <c r="O45" s="19"/>
       <c r="P45" s="19"/>
-      <c r="Q45" s="20"/>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q45" s="19"/>
+      <c r="R45" s="20"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="1" t="s">
         <v>26</v>
@@ -2520,9 +2622,10 @@
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
-      <c r="Q46" s="20"/>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q46" s="19"/>
+      <c r="R46" s="20"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="1" t="s">
         <v>27</v>
@@ -2540,9 +2643,10 @@
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
       <c r="P47" s="19"/>
-      <c r="Q47" s="20"/>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q47" s="19"/>
+      <c r="R47" s="20"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="23"/>
     </row>
   </sheetData>
@@ -2552,6 +2656,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100504F0EFF1BE61D46A34440DDC749B165" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6861fccdae819c068e3d2675729df3bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29ddf0ed-477c-451e-8755-cfaffaaa5733" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fc745dc185d8196f008ac861e10f643" ns2:_="">
     <xsd:import namespace="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
@@ -2683,22 +2802,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD7FEF4-E84B-468B-9D19-73896C646B9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2714,28 +2842,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KU5 - Updated Project plan. Gathered information and datasets on prototype
</commit_message>
<xml_diff>
--- a/doc/Project Plan_weekly.xlsx
+++ b/doc/Project Plan_weekly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\School\Semester2\Project\6.2A_MandyCortis_Project_Git\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE455114-6FBB-43A1-BE20-C0407C2FDB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B308DC-5D22-4A55-BC85-A08C084A25FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="9825" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
@@ -846,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37548FD9-318C-4A7A-9098-287F0A874FE1}">
   <dimension ref="B1:R49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62287C0-7FD6-48A5-9514-03B257F96545}">
   <dimension ref="B1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,25 +1914,6 @@
       <c r="Q7" s="19"/>
       <c r="R7" s="20"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="20"/>
-    </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
@@ -1993,8 +1974,8 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -2065,23 +2046,7 @@
       <c r="R15" s="20"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="20"/>
+      <c r="B16" s="23"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2194,23 +2159,7 @@
       <c r="R22" s="20"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="20"/>
+      <c r="B23" s="23"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2302,23 +2251,7 @@
       <c r="R28" s="20"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="20"/>
+      <c r="B29" s="23"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -2380,8 +2313,8 @@
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
@@ -2402,7 +2335,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
       <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
+      <c r="M34" s="10"/>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
@@ -2431,23 +2364,7 @@
       <c r="R35" s="20"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="20"/>
+      <c r="B36" s="23"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -2560,23 +2477,7 @@
       <c r="R42" s="20"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B43" s="5"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="20"/>
+      <c r="B43" s="23"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -2656,6 +2557,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100504F0EFF1BE61D46A34440DDC749B165" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6861fccdae819c068e3d2675729df3bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29ddf0ed-477c-451e-8755-cfaffaaa5733" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fc745dc185d8196f008ac861e10f643" ns2:_="">
     <xsd:import namespace="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
@@ -2787,22 +2703,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD7FEF4-E84B-468B-9D19-73896C646B9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2818,28 +2743,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>